<commit_message>
update and refresh runs
</commit_message>
<xml_diff>
--- a/PREPARE-TIMES-NZ/output/SuppXLS/Scen_Base_constraints.xlsx
+++ b/PREPARE-TIMES-NZ/output/SuppXLS/Scen_Base_constraints.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -431,283 +431,269 @@
     <row r="1">
       <c r="B1" t="inlineStr">
         <is>
-          <t xml:space="preserve">~UC_Sets: Ts_S: </t>
+          <t xml:space="preserve">~UC_Sets: T_SUC: </t>
         </is>
       </c>
     </row>
     <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>~UC_T</t>
+        </is>
+      </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">~UC_Sets: T_SUC: </t>
+          <t>~UC_Sets: R_S: AllRegions</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>~UC_T</t>
+          <t>UC_N</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>~UC_Sets: R_S: AllRegions</t>
+          <t>Pset_Set</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Pset_PN</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Pset_CI</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Pset_CO</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Cset_CN</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>UC_ATTR</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Year</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>LimType</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>UC_CAP</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>UC_CAP~RHS</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>UC_RHST</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>UC_RHST~0</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>UC_Desc</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>Max_BEVMTruck_uptake_number</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>T_F_MT*BEV*</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>CAP,GROWTH</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>LO</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>1.15</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>-17.5</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>Max number of BE medium trucks can be deployed per first year and next years</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">~UC_Sets: T_SUC: </t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>~UC_T</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>~UC_Sets: R_S: AllRegions</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
           <t>UC_N</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B9" t="inlineStr">
         <is>
           <t>Pset_Set</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>Pset_PN</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>Pset_CI</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>Pset_CO</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>Cset_CN</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>UC_ATTR</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>Year</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="I9" t="inlineStr">
         <is>
           <t>LimType</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="J9" t="inlineStr">
         <is>
           <t>UC_CAP</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>UC_CAP~RHS</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
+      <c r="K9" t="inlineStr">
         <is>
           <t>UC_RHST</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
+      <c r="L9" t="inlineStr">
         <is>
           <t>UC_RHST~0</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr">
+      <c r="M9" t="inlineStr">
         <is>
           <t>UC_Desc</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Max_BEVMTruck_uptake_number</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>T_F_MT*BEV*</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>CAP,GROWTH</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>LO</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>1.15</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>-17.5</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>Max number of BE medium trucks can be deployed per first year and next years</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">~UC_Sets: Ts_S: </t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">~UC_Sets: T_SUC: </t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>~UC_T</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>~UC_Sets: R_S: AllRegions</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>UC_N</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Pset_Set</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Pset_PN</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Pset_CI</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Pset_CO</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Cset_CN</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>UC_ATTR</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>Year</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>LimType</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>UC_CAP</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>UC_RHST</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>UC_RHST~0</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>UC_Desc</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
           <t>UC_BEV_BUS_limit</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>T_P_B*BEV*</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t>2016</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr">
+      <c r="I10" t="inlineStr">
         <is>
           <t>LO</t>
         </is>
       </c>
-      <c r="J12" t="inlineStr">
+      <c r="J10" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="K12" t="inlineStr">
+      <c r="K10" t="inlineStr">
         <is>
           <t>0.000721</t>
         </is>
       </c>
-      <c r="L12" t="inlineStr">
+      <c r="L10" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="M12" t="inlineStr">
+      <c r="M10" t="inlineStr">
         <is>
           <t>Minimal number of BE busses in the fleet</t>
         </is>

</xml_diff>

<commit_message>
first pass of new method
</commit_message>
<xml_diff>
--- a/PREPARE-TIMES-NZ/output/SuppXLS/Scen_Base_constraints.xlsx
+++ b/PREPARE-TIMES-NZ/output/SuppXLS/Scen_Base_constraints.xlsx
@@ -429,7 +429,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t xml:space="preserve">~UC_Sets: T_SUC: </t>
         </is>
@@ -438,12 +438,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>~UC_Sets: R_S: AllRegions</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>~UC_T</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>~UC_Sets: R_S: AllRegions</t>
         </is>
       </c>
     </row>
@@ -572,7 +572,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="B7" t="inlineStr">
+      <c r="A7" t="inlineStr">
         <is>
           <t xml:space="preserve">~UC_Sets: T_SUC: </t>
         </is>
@@ -581,12 +581,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>~UC_Sets: R_S: AllRegions</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>~UC_T</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>~UC_Sets: R_S: AllRegions</t>
         </is>
       </c>
     </row>
@@ -719,7 +719,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t xml:space="preserve">~UC_Sets: T_S: </t>
         </is>
@@ -728,12 +728,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>~UC_Sets: R_S: AllRegions</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>~UC_T</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>~UC_Sets: R_S: AllRegions</t>
         </is>
       </c>
     </row>
@@ -1659,7 +1659,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t xml:space="preserve">~UC_Sets: T_S: </t>
         </is>
@@ -1668,12 +1668,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>~UC_Sets: R_S: AllRegions</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>~UC_T</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>~UC_Sets: R_S: AllRegions</t>
         </is>
       </c>
     </row>
@@ -1833,7 +1833,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t xml:space="preserve">~UC_Sets: T_E: </t>
         </is>
@@ -1842,12 +1842,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>~UC_Sets: R_S: AllRegions</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>~UC_T</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>~UC_Sets: R_S: AllRegions</t>
         </is>
       </c>
     </row>
@@ -2017,7 +2017,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t xml:space="preserve">~UC_Sets: T_E: </t>
         </is>
@@ -2026,12 +2026,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>~UC_Sets: R_S: AllRegions</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>~UC_T</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>~UC_Sets: R_S: AllRegions</t>
         </is>
       </c>
     </row>
@@ -4568,7 +4568,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t xml:space="preserve">~UC_Sets: T_S: </t>
         </is>
@@ -4577,12 +4577,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>~UC_Sets: R_S: AllRegions</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>~TFM_INS</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>~UC_Sets: R_S: AllRegions</t>
         </is>
       </c>
     </row>
@@ -4802,7 +4802,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="B10" t="inlineStr">
+      <c r="A10" t="inlineStr">
         <is>
           <t xml:space="preserve">~UC_Sets: T_S: </t>
         </is>
@@ -4811,12 +4811,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>~UC_Sets: R_S: AllRegions</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
           <t>~TFM_UPD</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>~UC_Sets: R_S: AllRegions</t>
         </is>
       </c>
     </row>
@@ -4907,7 +4907,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="B17" t="inlineStr">
+      <c r="A17" t="inlineStr">
         <is>
           <t xml:space="preserve">~UC_Sets: T_S: </t>
         </is>
@@ -4916,12 +4916,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>~UC_Sets: R_S: AllRegions</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
           <t>~UC_T</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>~UC_Sets: R_S: AllRegions</t>
         </is>
       </c>
     </row>
@@ -5044,7 +5044,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t xml:space="preserve">~UC_Sets: T_E: </t>
         </is>
@@ -5053,12 +5053,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>~UC_Sets: R_E: AllRegions</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>~UC_T</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>~UC_Sets: R_E: AllRegions</t>
         </is>
       </c>
     </row>
@@ -5162,7 +5162,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="B7" t="inlineStr">
+      <c r="A7" t="inlineStr">
         <is>
           <t xml:space="preserve">~UC_Sets: T_E: </t>
         </is>
@@ -5171,12 +5171,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>~UC_Sets: R_E: AllRegions</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>~UC_T</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>~UC_Sets: R_E: AllRegions</t>
         </is>
       </c>
     </row>
@@ -5403,7 +5403,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t xml:space="preserve">~UC_Sets: T_E: </t>
         </is>
@@ -5412,12 +5412,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>~UC_Sets: R_E: AllRegions</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>~UC_T</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>~UC_Sets: R_E: AllRegions</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
reran recursively to ensure no additional information loss
</commit_message>
<xml_diff>
--- a/PREPARE-TIMES-NZ/output/SuppXLS/Scen_Base_constraints.xlsx
+++ b/PREPARE-TIMES-NZ/output/SuppXLS/Scen_Base_constraints.xlsx
@@ -431,14 +431,14 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t xml:space="preserve">~UC_Sets: T_SUC: </t>
+          <t>~UC_Sets: R_S: AllRegions</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>~UC_Sets: R_S: AllRegions</t>
+          <t xml:space="preserve">~UC_Sets: T_SUC: </t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -574,14 +574,14 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t xml:space="preserve">~UC_Sets: T_SUC: </t>
+          <t>~UC_Sets: R_S: AllRegions</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>~UC_Sets: R_S: AllRegions</t>
+          <t xml:space="preserve">~UC_Sets: T_SUC: </t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -721,14 +721,14 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t xml:space="preserve">~UC_Sets: T_S: </t>
+          <t>~UC_Sets: R_S: AllRegions</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>~UC_Sets: R_S: AllRegions</t>
+          <t xml:space="preserve">~UC_Sets: T_S: </t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1661,14 +1661,14 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t xml:space="preserve">~UC_Sets: T_S: </t>
+          <t>~UC_Sets: R_S: AllRegions</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>~UC_Sets: R_S: AllRegions</t>
+          <t xml:space="preserve">~UC_Sets: T_S: </t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1835,14 +1835,14 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t xml:space="preserve">~UC_Sets: T_E: </t>
+          <t>~UC_Sets: R_S: AllRegions</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>~UC_Sets: R_S: AllRegions</t>
+          <t xml:space="preserve">~UC_Sets: T_E: </t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -2019,14 +2019,14 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t xml:space="preserve">~UC_Sets: T_E: </t>
+          <t>~UC_Sets: R_S: AllRegions</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>~UC_Sets: R_S: AllRegions</t>
+          <t xml:space="preserve">~UC_Sets: T_E: </t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -4570,14 +4570,14 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t xml:space="preserve">~UC_Sets: T_S: </t>
+          <t>~UC_Sets: R_S: AllRegions</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>~UC_Sets: R_S: AllRegions</t>
+          <t xml:space="preserve">~UC_Sets: T_S: </t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -4804,14 +4804,14 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t xml:space="preserve">~UC_Sets: T_S: </t>
+          <t>~UC_Sets: R_S: AllRegions</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>~UC_Sets: R_S: AllRegions</t>
+          <t xml:space="preserve">~UC_Sets: T_S: </t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -4909,14 +4909,14 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t xml:space="preserve">~UC_Sets: T_S: </t>
+          <t>~UC_Sets: R_S: AllRegions</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>~UC_Sets: R_S: AllRegions</t>
+          <t xml:space="preserve">~UC_Sets: T_S: </t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -5046,14 +5046,14 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t xml:space="preserve">~UC_Sets: T_E: </t>
+          <t>~UC_Sets: R_E: AllRegions</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>~UC_Sets: R_E: AllRegions</t>
+          <t xml:space="preserve">~UC_Sets: T_E: </t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -5164,14 +5164,14 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t xml:space="preserve">~UC_Sets: T_E: </t>
+          <t>~UC_Sets: R_E: AllRegions</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>~UC_Sets: R_E: AllRegions</t>
+          <t xml:space="preserve">~UC_Sets: T_E: </t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -5405,14 +5405,14 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t xml:space="preserve">~UC_Sets: T_E: </t>
+          <t>~UC_Sets: R_E: AllRegions</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>~UC_Sets: R_E: AllRegions</t>
+          <t xml:space="preserve">~UC_Sets: T_E: </t>
         </is>
       </c>
       <c r="B2" t="inlineStr">

</xml_diff>